<commit_message>
Updated BOM (Ferrite Beads Link)
</commit_message>
<xml_diff>
--- a/BOM/1581.Enhanced.BOM.xlsx
+++ b/BOM/1581.Enhanced.BOM.xlsx
@@ -191,9 +191,6 @@
     <t>You can scavenge ferrite beads from virtually any dead Commodore device board.</t>
   </si>
   <si>
-    <t>https://www.ebay.com/itm/393879647053</t>
-  </si>
-  <si>
     <t>R1, R3, R9, R10, R11</t>
   </si>
   <si>
@@ -641,6 +638,9 @@
   </si>
   <si>
     <t>Resistor Network (alternate part)</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/173835843423</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1208,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1224,7 +1224,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1427,10 +1427,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
@@ -1496,8 +1496,8 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E19" s="2"/>
-      <c r="G19" s="3" t="s">
-        <v>56</v>
+      <c r="G19" s="13" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -1517,148 +1517,148 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
         <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
       </c>
       <c r="E21" s="2">
         <v>5</v>
       </c>
       <c r="F21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
       </c>
       <c r="E22" s="2">
         <v>4</v>
       </c>
       <c r="F22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="B23" t="s">
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="G23" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
         <v>69</v>
       </c>
-      <c r="B24" t="s">
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
         <v>73</v>
       </c>
-      <c r="B25" t="s">
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="2">
-        <v>1</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="G25" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E26" s="2"/>
       <c r="F26" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
         <v>79</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>80</v>
-      </c>
-      <c r="D27" t="s">
-        <v>81</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
       </c>
       <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="G28" s="13" t="s">
         <v>203</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s">
         <v>84</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
         <v>85</v>
       </c>
-      <c r="D29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="G29" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -1678,42 +1678,42 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" t="s">
         <v>88</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>89</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" s="2">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="2">
-        <v>1</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="G31" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="6"/>
       <c r="G32" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="M32" t="s">
         <v>96</v>
-      </c>
-      <c r="M32" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -1733,193 +1733,193 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" t="s">
         <v>98</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>99</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
         <v>100</v>
-      </c>
-      <c r="E34" s="2">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D35" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="G35" t="s">
         <v>103</v>
-      </c>
-      <c r="G35" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" t="s">
         <v>105</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="G36" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" t="s">
         <v>109</v>
       </c>
-      <c r="B37" t="s">
+      <c r="D37" t="s">
         <v>110</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G37" t="s">
         <v>111</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G37" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" t="s">
         <v>113</v>
       </c>
-      <c r="D38" t="s">
-        <v>114</v>
-      </c>
       <c r="E38" s="2">
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" t="s">
         <v>115</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>116</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" s="2">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
         <v>117</v>
       </c>
-      <c r="E39" s="2">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="G39" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" t="s">
         <v>120</v>
       </c>
-      <c r="D40" t="s">
-        <v>121</v>
-      </c>
       <c r="E40" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" t="s">
         <v>122</v>
       </c>
-      <c r="B41" t="s">
+      <c r="E41" s="2">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="E41" s="2">
-        <v>1</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G42" t="s">
         <v>103</v>
-      </c>
-      <c r="G42" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" t="s">
         <v>126</v>
       </c>
-      <c r="B43" t="s">
-        <v>127</v>
-      </c>
       <c r="E43" s="2">
         <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" t="s">
         <v>128</v>
       </c>
-      <c r="B44" t="s">
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
         <v>129</v>
       </c>
-      <c r="E44" s="2">
-        <v>1</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G44" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" t="s">
         <v>132</v>
       </c>
-      <c r="B45" t="s">
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
         <v>133</v>
       </c>
-      <c r="E45" s="2">
-        <v>1</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="G45" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" s="2">
         <v>7406</v>
@@ -1928,62 +1928,62 @@
         <v>2</v>
       </c>
       <c r="F46" t="s">
+        <v>136</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
       <c r="E47" s="2"/>
       <c r="G47" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" t="s">
         <v>140</v>
       </c>
-      <c r="B48" t="s">
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
         <v>141</v>
       </c>
-      <c r="E48" s="2">
-        <v>1</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="G48" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E49" s="2"/>
       <c r="G49" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" t="s">
         <v>145</v>
       </c>
-      <c r="B50" t="s">
+      <c r="E50" s="2">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
         <v>146</v>
       </c>
-      <c r="E50" s="2">
-        <v>1</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="G50" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B51" s="2">
         <v>7407</v>
@@ -1992,27 +1992,27 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
+        <v>149</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" t="s">
         <v>152</v>
       </c>
-      <c r="B52" t="s">
+      <c r="E52" s="2">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
         <v>153</v>
       </c>
-      <c r="E52" s="2">
-        <v>1</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="G52" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
@@ -2032,22 +2032,22 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" t="s">
         <v>156</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>157</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" s="2">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
         <v>158</v>
       </c>
-      <c r="E54" s="2">
-        <v>1</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="G54" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -2067,84 +2067,84 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>162</v>
+      </c>
+      <c r="B61" t="s">
         <v>163</v>
-      </c>
-      <c r="B61" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>165</v>
+      </c>
+      <c r="B64" t="s">
         <v>166</v>
-      </c>
-      <c r="B64" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B66" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B67" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>170</v>
+      </c>
+      <c r="B71" t="s">
         <v>171</v>
-      </c>
-      <c r="B71" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
@@ -2155,64 +2155,64 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B74" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D74" t="s">
+        <v>182</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" s="11" t="s">
         <v>183</v>
-      </c>
-      <c r="E74">
-        <v>1</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B75" t="s">
+        <v>180</v>
+      </c>
+      <c r="D75" t="s">
         <v>181</v>
       </c>
-      <c r="D75" t="s">
-        <v>182</v>
-      </c>
       <c r="E75">
         <v>1</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B76" t="s">
+        <v>185</v>
+      </c>
+      <c r="D76" t="s">
+        <v>181</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="D76" t="s">
-        <v>182</v>
-      </c>
-      <c r="E76">
-        <v>1</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>187</v>
+      </c>
+      <c r="B77" t="s">
         <v>188</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" t="s">
         <v>189</v>
-      </c>
-      <c r="D77" t="s">
-        <v>190</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -2220,7 +2220,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
@@ -2231,13 +2231,13 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>192</v>
+      </c>
+      <c r="B80" t="s">
         <v>193</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>194</v>
-      </c>
-      <c r="D80" t="s">
-        <v>195</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>195</v>
+      </c>
+      <c r="B81" t="s">
         <v>196</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>197</v>
-      </c>
-      <c r="D81" t="s">
-        <v>198</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -2259,13 +2259,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>198</v>
+      </c>
+      <c r="B82" t="s">
         <v>199</v>
       </c>
-      <c r="B82" t="s">
+      <c r="D82" t="s">
         <v>200</v>
-      </c>
-      <c r="D82" t="s">
-        <v>201</v>
       </c>
       <c r="E82">
         <v>1</v>

</xml_diff>